<commit_message>
Heading home from the library :)
</commit_message>
<xml_diff>
--- a/PROB_02_NL/LOAD_STEPS.xlsx
+++ b/PROB_02_NL/LOAD_STEPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage.it.tamu.edu\TAMU\OAL\Homes\tanmayeyashodan.h\AccountSettings\Desktop\ANALYSIS_OF_BEAMS\PROB_02_NL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B01D5FF-D724-421E-97B6-E71042EEA636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B666F0-7AFA-40AC-B401-B2507263E0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE15F2CF-35EA-4D23-B55B-62F87842D900}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="D4:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D15"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,8 @@
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <f>F6+1</f>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" ref="G7:G15" si="0">G6+D7</f>
@@ -488,7 +489,8 @@
         <v>1</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <f t="shared" ref="F8:F15" si="1">F7+1</f>
+        <v>3</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
@@ -500,7 +502,8 @@
         <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -512,7 +515,8 @@
         <v>1</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
@@ -524,7 +528,8 @@
         <v>1</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -536,7 +541,8 @@
         <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
@@ -548,7 +554,8 @@
         <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
@@ -560,7 +567,8 @@
         <v>1</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
@@ -572,7 +580,8 @@
         <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>

</xml_diff>